<commit_message>
:bug:fix bug in task2
</commit_message>
<xml_diff>
--- a/DisassembleData/Instruction_1900012739_.xlsx
+++ b/DisassembleData/Instruction_1900012739_.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="168">
   <si>
     <t>movq</t>
   </si>
@@ -514,13 +514,13 @@
     <t>双参指令</t>
   </si>
   <si>
+    <t>多参指令</t>
+  </si>
+  <si>
     <t>单参指令</t>
   </si>
   <si>
     <t>无参指令</t>
-  </si>
-  <si>
-    <t>多参指令</t>
   </si>
 </sst>
 </file>
@@ -2220,7 +2220,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2228,34 +2228,1314 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1">
-        <v>39254</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>165</v>
-      </c>
-      <c r="B2">
-        <v>19976</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3">
-        <v>1703</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>167</v>
       </c>
-      <c r="B4">
-        <v>281</v>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2290,7 +3570,7 @@
         <v>5769</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2312,7 +3592,7 @@
         <v>3453</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2323,7 +3603,7 @@
         <v>3332</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2345,7 +3625,7 @@
         <v>2645</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2356,7 +3636,7 @@
         <v>1907</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2367,7 +3647,7 @@
         <v>1444</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2444,7 +3724,7 @@
         <v>783</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2488,7 +3768,7 @@
         <v>585</v>
       </c>
       <c r="C20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2554,7 +3834,7 @@
         <v>311</v>
       </c>
       <c r="C26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2576,7 +3856,7 @@
         <v>276</v>
       </c>
       <c r="C28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2587,7 +3867,7 @@
         <v>252</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2598,7 +3878,7 @@
         <v>222</v>
       </c>
       <c r="C30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2653,7 +3933,7 @@
         <v>144</v>
       </c>
       <c r="C35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2664,7 +3944,7 @@
         <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2686,7 +3966,7 @@
         <v>139</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2708,7 +3988,7 @@
         <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2741,7 +4021,7 @@
         <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2763,7 +4043,7 @@
         <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2796,7 +4076,7 @@
         <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2807,7 +4087,7 @@
         <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2818,7 +4098,7 @@
         <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2862,7 +4142,7 @@
         <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2873,7 +4153,7 @@
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2917,7 +4197,7 @@
         <v>52</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2928,7 +4208,7 @@
         <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2939,7 +4219,7 @@
         <v>44</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2961,7 +4241,7 @@
         <v>41</v>
       </c>
       <c r="C63" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2972,7 +4252,7 @@
         <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2983,7 +4263,7 @@
         <v>38</v>
       </c>
       <c r="C65" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -3005,7 +4285,7 @@
         <v>32</v>
       </c>
       <c r="C67" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -3038,7 +4318,7 @@
         <v>30</v>
       </c>
       <c r="C70" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -3060,7 +4340,7 @@
         <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -3126,7 +4406,7 @@
         <v>23</v>
       </c>
       <c r="C78" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -3137,7 +4417,7 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -3170,7 +4450,7 @@
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -3181,7 +4461,7 @@
         <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -3192,7 +4472,7 @@
         <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -3225,7 +4505,7 @@
         <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -3247,7 +4527,7 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -3280,7 +4560,7 @@
         <v>11</v>
       </c>
       <c r="C92" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -3291,7 +4571,7 @@
         <v>11</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -3302,7 +4582,7 @@
         <v>11</v>
       </c>
       <c r="C94" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -3335,7 +4615,7 @@
         <v>7</v>
       </c>
       <c r="C97" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -3357,7 +4637,7 @@
         <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -3390,7 +4670,7 @@
         <v>7</v>
       </c>
       <c r="C102" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -3478,7 +4758,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -3489,7 +4769,7 @@
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -3500,7 +4780,7 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -3511,7 +4791,7 @@
         <v>4</v>
       </c>
       <c r="C113" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3522,7 +4802,7 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3555,7 +4835,7 @@
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3566,7 +4846,7 @@
         <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3577,7 +4857,7 @@
         <v>3</v>
       </c>
       <c r="C119" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3588,7 +4868,7 @@
         <v>3</v>
       </c>
       <c r="C120" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -3610,7 +4890,7 @@
         <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -3643,7 +4923,7 @@
         <v>2</v>
       </c>
       <c r="C125" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3654,7 +4934,7 @@
         <v>2</v>
       </c>
       <c r="C126" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -3665,7 +4945,7 @@
         <v>2</v>
       </c>
       <c r="C127" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -3742,7 +5022,7 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -3808,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3830,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -3852,7 +5132,7 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3874,7 +5154,7 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3885,7 +5165,7 @@
         <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -3896,7 +5176,7 @@
         <v>1</v>
       </c>
       <c r="C148" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3918,7 +5198,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3929,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -4017,7 +5297,7 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -4050,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="C162" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -4061,7 +5341,7 @@
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -4072,7 +5352,7 @@
         <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>